<commit_message>
modified code to add filter code which will remove or don't give companies that dont offer sponsorship
</commit_message>
<xml_diff>
--- a/Output/found_jobs.xlsx
+++ b/Output/found_jobs.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -451,13 +451,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <cols>
+    <col width="50.19921875" customWidth="1" min="1" max="1"/>
+    <col width="46.265625" customWidth="1" min="2" max="2"/>
+    <col width="32.86328125" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1233,7 +1238,6 @@
           <t>Redhorse Corp</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
           <t>Virginia</t>
@@ -1261,7 +1265,6 @@
           <t>Brandstetter Carroll Inc.</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
           <t>Ohio</t>
@@ -1718,6 +1721,286 @@
       <c r="F40" t="inlineStr">
         <is>
           <t>https://southbeachastorianyc.com/wp-job/job/entry-level-cloud-data-engineer-at-synergisticit-seattle-wa-RU5EVDZDOTgzVDlSSjhuWXJwUlpVYlpwOFE9PQ==?utm_campaign=google_jobs_apply&amp;utm_source=google_jobs_apply&amp;utm_medium=organic</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>gXGih_3idtegO6LOAAAAAA==</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Entry Level QA (H1b Visa Sponsorship Available)</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Perfict Global, Inc.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://www.optnation.com/entry-level-qa-h1b-visa-sponsorship-available-job-in-new-york-ny-view-jobid-33407?utm_campaign=google_jobs_apply&amp;utm_source=google_jobs_apply&amp;utm_medium=organic</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Allows: explicit sponsorship signal ('Visa Sponsorship')</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>dh3Ad6iNO2ZMLcIBAAAAAA==</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Training&amp;Placement in Business Analyst along with certification|VISA Sponsorship</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>PrecisionTechnologies Corp</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>South Brunswick Township</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>New Jersey</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>https://applicant.mightyrecruiter.com/jobs/apply/training-placement-in-business-analyst-along-with-certification-visa-sponsorship-at-precisiontechnologies-corp-in-south-brunswick-township-nj-e35475dc6941c5c2f182ca3f2182b448?utm_campaign=google_jobs_apply&amp;utm_source=google_jobs_apply&amp;utm_medium=organic</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Allows: explicit sponsorship signal ('VISA Sponsorship')</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>pUeEVpkGzM8fAmDyAAAAAA==</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>QA Analyst (H1b Visa Sponsorship Available)</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Perfict Global, Inc.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Boston</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Massachusetts</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>https://www.optnation.com/qa-analyst-h1b-visa-sponsorship-available-job-in-boston-ma-view-jobid-33582?utm_campaign=google_jobs_apply&amp;utm_source=google_jobs_apply&amp;utm_medium=organic</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Allows: explicit sponsorship signal ('Visa Sponsorship')</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>eZczUsY6W1vQHTaGAAAAAA==</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Entry Level QA (H1b Visa Sponsorship Available)</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Perfict Global, Inc.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Pittsburgh</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Pennsylvania</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>https://www.optnation.com/entry-level-qa-h1b-visa-sponsorship-available-job-in-pittsburgh-pa-view-jobid-33580?utm_campaign=google_jobs_apply&amp;utm_source=google_jobs_apply&amp;utm_medium=organic</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Allows: explicit sponsorship signal ('Visa Sponsorship')</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>xoM74PXhUYkigicIAAAAAA==</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Entry Level QA (H1b Visa Sponsorship Available)</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Perfict Global, Inc.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Louisville</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Kentucky</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://www.optnation.com/entry-level-qa-h1b-visa-sponsorship-available-job-in-louisville-ky-view-jobid-33765?utm_campaign=google_jobs_apply&amp;utm_source=google_jobs_apply&amp;utm_medium=organic</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Allows: explicit sponsorship signal ('Visa Sponsorship')</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>yv24shpMgCVxcssFAAAAAA==</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Junior Software Developer – USA Visa Sponsorship in USA – (job id: 1681772381)</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>vmysmartpros</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://www.mysmartpros.com/tuition/job/junior-software-developer-usa-visa-sponsorship-in-usa-job-id-1681772381/?utm_campaign=google_jobs_apply&amp;utm_source=google_jobs_apply&amp;utm_medium=organic</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Allows: explicit sponsorship signal ('Visa Sponsorship')</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>4vszmTyq5cJb08j9AAAAAA==</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Entry Level Software Tester (H1b Visa Sponsorship available)</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>athomejobs5.10001mb</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://athomejobs5.10001mb.com/job/entry-level-software-tester-h1b-visa-sponsorship-available?utm_campaign=google_jobs_apply&amp;utm_source=google_jobs_apply&amp;utm_medium=organic</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Allows: explicit sponsorship signal ('Visa Sponsorship')</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>KYU9wwLCb_wuuemFAAAAAA==</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Data Engineer at BeaconFire Inc. Trenton, NJ</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>BeaconFire Inc.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Trenton</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>New Jersey</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://badidearadio.com/job-library/job/data-engineer-at-beaconfire-inc-trenton-nj-a05vcmNiRC9JbEl1VkJJelhXYWN1aHpUeVE9PQ==?utm_campaign=google_jobs_apply&amp;utm_source=google_jobs_apply&amp;utm_medium=organic</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Allows: explicit sponsorship signal ('visa sponsorship')</t>
         </is>
       </c>
     </row>

</xml_diff>